<commit_message>
DMP-460 add test, and fix test data
</commit_message>
<xml_diff>
--- a/testDataHelper.xlsx
+++ b/testDataHelper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrismagowan/Documents/code/darts-api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4506154C-0F6D-574B-8F89-3F2BA9FC2416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF3622D-0CFA-714A-AD91-3A6D424F46C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21800" xr2:uid="{28D61736-E8C7-5248-BA7C-21A030F87339}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve"> r_case_object_id</t>
   </si>
   <si>
-    <t xml:space="preserve"> c_type</t>
-  </si>
-  <si>
     <t xml:space="preserve"> c_case_id</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve"> r_version_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> i_superseded</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> i_version</t>
   </si>
 </sst>
 </file>
@@ -456,7 +447,8 @@
   <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K161" sqref="K2:K161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2291,7 +2283,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E66" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F66" s="1">
         <v>0.375</v>
@@ -2301,7 +2293,7 @@
       </c>
       <c r="K66" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO moj_hearing VALUES (65,1,1,'{Judge1}','2023-06-21','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (65,1,1,'{Judge1}','2023-06-22','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2319,7 +2311,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E67" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F67" s="1">
         <v>0.41666666666666669</v>
@@ -2329,7 +2321,7 @@
       </c>
       <c r="K67" t="str">
         <f t="shared" ref="K67:K130" si="2">"INSERT INTO moj_hearing VALUES ("&amp;A67&amp;","&amp;B67&amp;","&amp;C67&amp;",'"&amp;D67&amp;"','"&amp;TEXT(E67,"yyyy-MM-dd")&amp;"','"&amp;TEXT(F67,"HH:mm:ss")&amp;"',"&amp;G67&amp;", NULL);"</f>
-        <v>INSERT INTO moj_hearing VALUES (66,2,1,'{Judge1}','2023-06-21','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (66,2,1,'{Judge1}','2023-06-22','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2347,7 +2339,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E68" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F68" s="1">
         <v>0.45833333333333331</v>
@@ -2357,7 +2349,7 @@
       </c>
       <c r="K68" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (67,3,1,'{Judge1}','2023-06-21','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (67,3,1,'{Judge1}','2023-06-22','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -2375,7 +2367,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E69" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F69" s="1">
         <v>0.5</v>
@@ -2385,7 +2377,7 @@
       </c>
       <c r="K69" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (68,4,1,'{Judge1}','2023-06-21','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (68,4,1,'{Judge1}','2023-06-22','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -2403,7 +2395,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E70" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F70" s="1">
         <v>0.54166666666666696</v>
@@ -2413,7 +2405,7 @@
       </c>
       <c r="K70" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (69,5,1,'{Judge1}','2023-06-21','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (69,5,1,'{Judge1}','2023-06-22','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2431,7 +2423,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E71" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F71" s="1">
         <v>0.58333333333333404</v>
@@ -2441,7 +2433,7 @@
       </c>
       <c r="K71" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (70,6,1,'{Judge1}','2023-06-21','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (70,6,1,'{Judge1}','2023-06-22','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -2459,7 +2451,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E72" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F72" s="1">
         <v>0.625</v>
@@ -2469,7 +2461,7 @@
       </c>
       <c r="K72" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (71,7,1,'{Judge1}','2023-06-21','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (71,7,1,'{Judge1}','2023-06-22','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -2487,7 +2479,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E73" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F73" s="1">
         <v>0.66666666666666696</v>
@@ -2497,7 +2489,7 @@
       </c>
       <c r="K73" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (72,8,1,'{Judge1}','2023-06-21','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (72,8,1,'{Judge1}','2023-06-22','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -2515,7 +2507,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E74" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F74" s="1">
         <v>0.375</v>
@@ -2525,7 +2517,7 @@
       </c>
       <c r="K74" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (73,9,2,'{Judge2}','2023-06-21','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (73,9,2,'{Judge2}','2023-06-22','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -2543,7 +2535,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E75" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F75" s="1">
         <v>0.41666666666666669</v>
@@ -2553,7 +2545,7 @@
       </c>
       <c r="K75" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (74,10,2,'{Judge2}','2023-06-21','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (74,10,2,'{Judge2}','2023-06-22','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -2571,7 +2563,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E76" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F76" s="1">
         <v>0.45833333333333331</v>
@@ -2581,7 +2573,7 @@
       </c>
       <c r="K76" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (75,11,2,'{Judge2}','2023-06-21','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (75,11,2,'{Judge2}','2023-06-22','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -2599,7 +2591,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E77" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F77" s="1">
         <v>0.5</v>
@@ -2609,7 +2601,7 @@
       </c>
       <c r="K77" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (76,12,2,'{Judge2}','2023-06-21','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (76,12,2,'{Judge2}','2023-06-22','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -2627,7 +2619,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E78" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F78" s="1">
         <v>0.54166666666666696</v>
@@ -2637,7 +2629,7 @@
       </c>
       <c r="K78" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (77,13,2,'{Judge2}','2023-06-21','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (77,13,2,'{Judge2}','2023-06-22','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -2655,7 +2647,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E79" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F79" s="1">
         <v>0.58333333333333404</v>
@@ -2665,7 +2657,7 @@
       </c>
       <c r="K79" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (78,14,2,'{Judge2}','2023-06-21','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (78,14,2,'{Judge2}','2023-06-22','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -2683,7 +2675,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E80" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F80" s="1">
         <v>0.625</v>
@@ -2693,7 +2685,7 @@
       </c>
       <c r="K80" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (79,15,2,'{Judge2}','2023-06-21','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (79,15,2,'{Judge2}','2023-06-22','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -2711,7 +2703,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E81" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F81" s="1">
         <v>0.66666666666666696</v>
@@ -2721,7 +2713,7 @@
       </c>
       <c r="K81" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (80,16,2,'{Judge2}','2023-06-21','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (80,16,2,'{Judge2}','2023-06-22','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -2739,7 +2731,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E82" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F82" s="1">
         <v>0.375</v>
@@ -2749,7 +2741,7 @@
       </c>
       <c r="K82" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (81,17,3,'{Judge3}','2023-06-21','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (81,17,3,'{Judge3}','2023-06-22','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -2767,7 +2759,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E83" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F83" s="1">
         <v>0.41666666666666669</v>
@@ -2777,7 +2769,7 @@
       </c>
       <c r="K83" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (82,18,3,'{Judge3}','2023-06-21','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (82,18,3,'{Judge3}','2023-06-22','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -2795,7 +2787,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E84" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F84" s="1">
         <v>0.45833333333333331</v>
@@ -2805,7 +2797,7 @@
       </c>
       <c r="K84" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (83,19,3,'{Judge3}','2023-06-21','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (83,19,3,'{Judge3}','2023-06-22','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -2823,7 +2815,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E85" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F85" s="1">
         <v>0.5</v>
@@ -2833,7 +2825,7 @@
       </c>
       <c r="K85" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (84,20,3,'{Judge3}','2023-06-21','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (84,20,3,'{Judge3}','2023-06-22','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -2851,7 +2843,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E86" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F86" s="1">
         <v>0.54166666666666696</v>
@@ -2861,7 +2853,7 @@
       </c>
       <c r="K86" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (85,21,3,'{Judge3}','2023-06-21','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (85,21,3,'{Judge3}','2023-06-22','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -2879,7 +2871,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E87" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F87" s="1">
         <v>0.58333333333333404</v>
@@ -2889,7 +2881,7 @@
       </c>
       <c r="K87" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (86,22,3,'{Judge3}','2023-06-21','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (86,22,3,'{Judge3}','2023-06-22','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
@@ -2907,7 +2899,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E88" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F88" s="1">
         <v>0.625</v>
@@ -2917,7 +2909,7 @@
       </c>
       <c r="K88" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (87,23,3,'{Judge3}','2023-06-21','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (87,23,3,'{Judge3}','2023-06-22','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
@@ -2935,7 +2927,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E89" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F89" s="1">
         <v>0.66666666666666696</v>
@@ -2945,7 +2937,7 @@
       </c>
       <c r="K89" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (88,24,3,'{Judge3}','2023-06-21','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (88,24,3,'{Judge3}','2023-06-22','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -2963,7 +2955,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E90" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F90" s="1">
         <v>0.375</v>
@@ -2973,7 +2965,7 @@
       </c>
       <c r="K90" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (89,25,4,'{Judge4}','2023-06-21','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (89,25,4,'{Judge4}','2023-06-22','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -2991,7 +2983,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E91" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F91" s="1">
         <v>0.41666666666666669</v>
@@ -3001,7 +2993,7 @@
       </c>
       <c r="K91" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (90,26,4,'{Judge4}','2023-06-21','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (90,26,4,'{Judge4}','2023-06-22','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -3019,7 +3011,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E92" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F92" s="1">
         <v>0.45833333333333331</v>
@@ -3029,7 +3021,7 @@
       </c>
       <c r="K92" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (91,27,4,'{Judge4}','2023-06-21','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (91,27,4,'{Judge4}','2023-06-22','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -3047,7 +3039,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E93" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F93" s="1">
         <v>0.5</v>
@@ -3057,7 +3049,7 @@
       </c>
       <c r="K93" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (92,28,4,'{Judge4}','2023-06-21','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (92,28,4,'{Judge4}','2023-06-22','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -3075,7 +3067,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E94" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F94" s="1">
         <v>0.54166666666666696</v>
@@ -3085,7 +3077,7 @@
       </c>
       <c r="K94" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (93,29,4,'{Judge4}','2023-06-21','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (93,29,4,'{Judge4}','2023-06-22','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -3103,7 +3095,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E95" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F95" s="1">
         <v>0.58333333333333404</v>
@@ -3113,7 +3105,7 @@
       </c>
       <c r="K95" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (94,30,4,'{Judge4}','2023-06-21','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (94,30,4,'{Judge4}','2023-06-22','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -3131,7 +3123,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E96" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F96" s="1">
         <v>0.625</v>
@@ -3141,7 +3133,7 @@
       </c>
       <c r="K96" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (95,31,4,'{Judge4}','2023-06-21','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (95,31,4,'{Judge4}','2023-06-22','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -3159,7 +3151,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E97" s="2">
-        <v>45098</v>
+        <v>45099</v>
       </c>
       <c r="F97" s="1">
         <v>0.66666666666666696</v>
@@ -3169,7 +3161,7 @@
       </c>
       <c r="K97" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (96,32,4,'{Judge4}','2023-06-21','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (96,32,4,'{Judge4}','2023-06-22','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -3187,7 +3179,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E98" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F98" s="1">
         <v>0.375</v>
@@ -3197,7 +3189,7 @@
       </c>
       <c r="K98" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (97,1,1,'{Judge1}','2023-06-22','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (97,1,1,'{Judge1}','2023-06-23','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -3215,7 +3207,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E99" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F99" s="1">
         <v>0.41666666666666669</v>
@@ -3225,7 +3217,7 @@
       </c>
       <c r="K99" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (98,2,1,'{Judge1}','2023-06-22','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (98,2,1,'{Judge1}','2023-06-23','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -3243,7 +3235,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E100" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F100" s="1">
         <v>0.45833333333333331</v>
@@ -3253,7 +3245,7 @@
       </c>
       <c r="K100" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (99,3,1,'{Judge1}','2023-06-22','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (99,3,1,'{Judge1}','2023-06-23','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -3271,7 +3263,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E101" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F101" s="1">
         <v>0.5</v>
@@ -3281,7 +3273,7 @@
       </c>
       <c r="K101" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (100,4,1,'{Judge1}','2023-06-22','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (100,4,1,'{Judge1}','2023-06-23','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
@@ -3299,7 +3291,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E102" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F102" s="1">
         <v>0.54166666666666696</v>
@@ -3309,7 +3301,7 @@
       </c>
       <c r="K102" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (101,5,1,'{Judge1}','2023-06-22','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (101,5,1,'{Judge1}','2023-06-23','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -3327,7 +3319,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E103" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F103" s="1">
         <v>0.58333333333333404</v>
@@ -3337,7 +3329,7 @@
       </c>
       <c r="K103" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (102,6,1,'{Judge1}','2023-06-22','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (102,6,1,'{Judge1}','2023-06-23','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
@@ -3355,7 +3347,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E104" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F104" s="1">
         <v>0.625</v>
@@ -3365,7 +3357,7 @@
       </c>
       <c r="K104" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (103,7,1,'{Judge1}','2023-06-22','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (103,7,1,'{Judge1}','2023-06-23','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -3383,7 +3375,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E105" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F105" s="1">
         <v>0.66666666666666696</v>
@@ -3393,7 +3385,7 @@
       </c>
       <c r="K105" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (104,8,1,'{Judge1}','2023-06-22','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (104,8,1,'{Judge1}','2023-06-23','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -3411,7 +3403,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E106" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F106" s="1">
         <v>0.375</v>
@@ -3421,7 +3413,7 @@
       </c>
       <c r="K106" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (105,9,2,'{Judge2}','2023-06-22','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (105,9,2,'{Judge2}','2023-06-23','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -3439,7 +3431,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E107" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F107" s="1">
         <v>0.41666666666666669</v>
@@ -3449,7 +3441,7 @@
       </c>
       <c r="K107" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (106,10,2,'{Judge2}','2023-06-22','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (106,10,2,'{Judge2}','2023-06-23','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -3467,7 +3459,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E108" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F108" s="1">
         <v>0.45833333333333331</v>
@@ -3477,7 +3469,7 @@
       </c>
       <c r="K108" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (107,11,2,'{Judge2}','2023-06-22','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (107,11,2,'{Judge2}','2023-06-23','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -3495,7 +3487,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E109" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F109" s="1">
         <v>0.5</v>
@@ -3505,7 +3497,7 @@
       </c>
       <c r="K109" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (108,12,2,'{Judge2}','2023-06-22','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (108,12,2,'{Judge2}','2023-06-23','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -3523,7 +3515,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E110" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F110" s="1">
         <v>0.54166666666666696</v>
@@ -3533,7 +3525,7 @@
       </c>
       <c r="K110" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (109,13,2,'{Judge2}','2023-06-22','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (109,13,2,'{Judge2}','2023-06-23','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -3551,7 +3543,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E111" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F111" s="1">
         <v>0.58333333333333404</v>
@@ -3561,7 +3553,7 @@
       </c>
       <c r="K111" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (110,14,2,'{Judge2}','2023-06-22','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (110,14,2,'{Judge2}','2023-06-23','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
@@ -3579,7 +3571,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E112" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F112" s="1">
         <v>0.625</v>
@@ -3589,7 +3581,7 @@
       </c>
       <c r="K112" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (111,15,2,'{Judge2}','2023-06-22','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (111,15,2,'{Judge2}','2023-06-23','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
@@ -3607,7 +3599,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E113" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F113" s="1">
         <v>0.66666666666666696</v>
@@ -3617,7 +3609,7 @@
       </c>
       <c r="K113" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (112,16,2,'{Judge2}','2023-06-22','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (112,16,2,'{Judge2}','2023-06-23','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
@@ -3635,7 +3627,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E114" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F114" s="1">
         <v>0.375</v>
@@ -3645,7 +3637,7 @@
       </c>
       <c r="K114" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (113,17,3,'{Judge3}','2023-06-22','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (113,17,3,'{Judge3}','2023-06-23','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
@@ -3663,7 +3655,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E115" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F115" s="1">
         <v>0.41666666666666669</v>
@@ -3673,7 +3665,7 @@
       </c>
       <c r="K115" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (114,18,3,'{Judge3}','2023-06-22','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (114,18,3,'{Judge3}','2023-06-23','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -3691,7 +3683,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E116" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F116" s="1">
         <v>0.45833333333333331</v>
@@ -3701,7 +3693,7 @@
       </c>
       <c r="K116" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (115,19,3,'{Judge3}','2023-06-22','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (115,19,3,'{Judge3}','2023-06-23','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -3719,7 +3711,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E117" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F117" s="1">
         <v>0.5</v>
@@ -3729,7 +3721,7 @@
       </c>
       <c r="K117" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (116,20,3,'{Judge3}','2023-06-22','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (116,20,3,'{Judge3}','2023-06-23','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -3747,7 +3739,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E118" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F118" s="1">
         <v>0.54166666666666696</v>
@@ -3757,7 +3749,7 @@
       </c>
       <c r="K118" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (117,21,3,'{Judge3}','2023-06-22','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (117,21,3,'{Judge3}','2023-06-23','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
@@ -3775,7 +3767,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E119" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F119" s="1">
         <v>0.58333333333333404</v>
@@ -3785,7 +3777,7 @@
       </c>
       <c r="K119" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (118,22,3,'{Judge3}','2023-06-22','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (118,22,3,'{Judge3}','2023-06-23','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
@@ -3803,7 +3795,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E120" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F120" s="1">
         <v>0.625</v>
@@ -3813,7 +3805,7 @@
       </c>
       <c r="K120" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (119,23,3,'{Judge3}','2023-06-22','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (119,23,3,'{Judge3}','2023-06-23','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
@@ -3831,7 +3823,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E121" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F121" s="1">
         <v>0.66666666666666696</v>
@@ -3841,7 +3833,7 @@
       </c>
       <c r="K121" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (120,24,3,'{Judge3}','2023-06-22','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (120,24,3,'{Judge3}','2023-06-23','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -3859,7 +3851,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E122" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F122" s="1">
         <v>0.375</v>
@@ -3869,7 +3861,7 @@
       </c>
       <c r="K122" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (121,25,4,'{Judge4}','2023-06-22','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (121,25,4,'{Judge4}','2023-06-23','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
@@ -3887,7 +3879,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E123" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F123" s="1">
         <v>0.41666666666666669</v>
@@ -3897,7 +3889,7 @@
       </c>
       <c r="K123" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (122,26,4,'{Judge4}','2023-06-22','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (122,26,4,'{Judge4}','2023-06-23','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
@@ -3915,7 +3907,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E124" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F124" s="1">
         <v>0.45833333333333331</v>
@@ -3925,7 +3917,7 @@
       </c>
       <c r="K124" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (123,27,4,'{Judge4}','2023-06-22','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (123,27,4,'{Judge4}','2023-06-23','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
@@ -3943,7 +3935,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E125" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F125" s="1">
         <v>0.5</v>
@@ -3953,7 +3945,7 @@
       </c>
       <c r="K125" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (124,28,4,'{Judge4}','2023-06-22','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (124,28,4,'{Judge4}','2023-06-23','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -3971,7 +3963,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E126" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F126" s="1">
         <v>0.54166666666666696</v>
@@ -3981,7 +3973,7 @@
       </c>
       <c r="K126" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (125,29,4,'{Judge4}','2023-06-22','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (125,29,4,'{Judge4}','2023-06-23','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
@@ -3999,7 +3991,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E127" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F127" s="1">
         <v>0.58333333333333404</v>
@@ -4009,7 +4001,7 @@
       </c>
       <c r="K127" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (126,30,4,'{Judge4}','2023-06-22','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (126,30,4,'{Judge4}','2023-06-23','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
@@ -4027,7 +4019,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E128" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F128" s="1">
         <v>0.625</v>
@@ -4037,7 +4029,7 @@
       </c>
       <c r="K128" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (127,31,4,'{Judge4}','2023-06-22','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (127,31,4,'{Judge4}','2023-06-23','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
@@ -4055,7 +4047,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E129" s="2">
-        <v>45099</v>
+        <v>45100</v>
       </c>
       <c r="F129" s="1">
         <v>0.66666666666666696</v>
@@ -4065,7 +4057,7 @@
       </c>
       <c r="K129" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (128,32,4,'{Judge4}','2023-06-22','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (128,32,4,'{Judge4}','2023-06-23','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
@@ -4083,7 +4075,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E130" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F130" s="1">
         <v>0.375</v>
@@ -4093,7 +4085,7 @@
       </c>
       <c r="K130" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO moj_hearing VALUES (129,1,1,'{Judge1}','2023-06-23','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (129,1,1,'{Judge1}','2023-06-24','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
@@ -4111,7 +4103,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E131" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F131" s="1">
         <v>0.41666666666666669</v>
@@ -4121,7 +4113,7 @@
       </c>
       <c r="K131" t="str">
         <f t="shared" ref="K131:K161" si="6">"INSERT INTO moj_hearing VALUES ("&amp;A131&amp;","&amp;B131&amp;","&amp;C131&amp;",'"&amp;D131&amp;"','"&amp;TEXT(E131,"yyyy-MM-dd")&amp;"','"&amp;TEXT(F131,"HH:mm:ss")&amp;"',"&amp;G131&amp;", NULL);"</f>
-        <v>INSERT INTO moj_hearing VALUES (130,2,1,'{Judge1}','2023-06-23','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (130,2,1,'{Judge1}','2023-06-24','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
@@ -4139,7 +4131,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E132" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F132" s="1">
         <v>0.45833333333333331</v>
@@ -4149,7 +4141,7 @@
       </c>
       <c r="K132" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (131,3,1,'{Judge1}','2023-06-23','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (131,3,1,'{Judge1}','2023-06-24','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
@@ -4167,7 +4159,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E133" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F133" s="1">
         <v>0.5</v>
@@ -4177,7 +4169,7 @@
       </c>
       <c r="K133" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (132,4,1,'{Judge1}','2023-06-23','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (132,4,1,'{Judge1}','2023-06-24','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
@@ -4195,7 +4187,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E134" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F134" s="1">
         <v>0.54166666666666696</v>
@@ -4205,7 +4197,7 @@
       </c>
       <c r="K134" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (133,5,1,'{Judge1}','2023-06-23','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (133,5,1,'{Judge1}','2023-06-24','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
@@ -4223,7 +4215,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E135" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F135" s="1">
         <v>0.58333333333333404</v>
@@ -4233,7 +4225,7 @@
       </c>
       <c r="K135" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (134,6,1,'{Judge1}','2023-06-23','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (134,6,1,'{Judge1}','2023-06-24','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
@@ -4251,7 +4243,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E136" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F136" s="1">
         <v>0.625</v>
@@ -4261,7 +4253,7 @@
       </c>
       <c r="K136" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (135,7,1,'{Judge1}','2023-06-23','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (135,7,1,'{Judge1}','2023-06-24','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
@@ -4279,7 +4271,7 @@
         <v>{Judge1}</v>
       </c>
       <c r="E137" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F137" s="1">
         <v>0.66666666666666696</v>
@@ -4289,7 +4281,7 @@
       </c>
       <c r="K137" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (136,8,1,'{Judge1}','2023-06-23','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (136,8,1,'{Judge1}','2023-06-24','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
@@ -4307,7 +4299,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E138" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F138" s="1">
         <v>0.375</v>
@@ -4317,7 +4309,7 @@
       </c>
       <c r="K138" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (137,9,2,'{Judge2}','2023-06-23','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (137,9,2,'{Judge2}','2023-06-24','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -4335,7 +4327,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E139" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F139" s="1">
         <v>0.41666666666666669</v>
@@ -4345,7 +4337,7 @@
       </c>
       <c r="K139" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (138,10,2,'{Judge2}','2023-06-23','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (138,10,2,'{Judge2}','2023-06-24','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
@@ -4363,7 +4355,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E140" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F140" s="1">
         <v>0.45833333333333331</v>
@@ -4373,7 +4365,7 @@
       </c>
       <c r="K140" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (139,11,2,'{Judge2}','2023-06-23','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (139,11,2,'{Judge2}','2023-06-24','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
@@ -4391,7 +4383,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E141" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F141" s="1">
         <v>0.5</v>
@@ -4401,7 +4393,7 @@
       </c>
       <c r="K141" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (140,12,2,'{Judge2}','2023-06-23','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (140,12,2,'{Judge2}','2023-06-24','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
@@ -4419,7 +4411,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E142" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F142" s="1">
         <v>0.54166666666666696</v>
@@ -4429,7 +4421,7 @@
       </c>
       <c r="K142" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (141,13,2,'{Judge2}','2023-06-23','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (141,13,2,'{Judge2}','2023-06-24','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
@@ -4447,7 +4439,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E143" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F143" s="1">
         <v>0.58333333333333404</v>
@@ -4457,7 +4449,7 @@
       </c>
       <c r="K143" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (142,14,2,'{Judge2}','2023-06-23','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (142,14,2,'{Judge2}','2023-06-24','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.2">
@@ -4475,7 +4467,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E144" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F144" s="1">
         <v>0.625</v>
@@ -4485,7 +4477,7 @@
       </c>
       <c r="K144" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (143,15,2,'{Judge2}','2023-06-23','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (143,15,2,'{Judge2}','2023-06-24','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
@@ -4503,7 +4495,7 @@
         <v>{Judge2}</v>
       </c>
       <c r="E145" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F145" s="1">
         <v>0.66666666666666696</v>
@@ -4513,7 +4505,7 @@
       </c>
       <c r="K145" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (144,16,2,'{Judge2}','2023-06-23','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (144,16,2,'{Judge2}','2023-06-24','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
@@ -4531,7 +4523,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E146" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F146" s="1">
         <v>0.375</v>
@@ -4541,7 +4533,7 @@
       </c>
       <c r="K146" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (145,17,3,'{Judge3}','2023-06-23','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (145,17,3,'{Judge3}','2023-06-24','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
@@ -4559,7 +4551,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E147" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F147" s="1">
         <v>0.41666666666666669</v>
@@ -4569,7 +4561,7 @@
       </c>
       <c r="K147" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (146,18,3,'{Judge3}','2023-06-23','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (146,18,3,'{Judge3}','2023-06-24','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
@@ -4587,7 +4579,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E148" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F148" s="1">
         <v>0.45833333333333331</v>
@@ -4597,7 +4589,7 @@
       </c>
       <c r="K148" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (147,19,3,'{Judge3}','2023-06-23','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (147,19,3,'{Judge3}','2023-06-24','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
@@ -4615,7 +4607,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E149" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F149" s="1">
         <v>0.5</v>
@@ -4625,7 +4617,7 @@
       </c>
       <c r="K149" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (148,20,3,'{Judge3}','2023-06-23','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (148,20,3,'{Judge3}','2023-06-24','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
@@ -4643,7 +4635,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E150" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F150" s="1">
         <v>0.54166666666666696</v>
@@ -4653,7 +4645,7 @@
       </c>
       <c r="K150" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (149,21,3,'{Judge3}','2023-06-23','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (149,21,3,'{Judge3}','2023-06-24','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
@@ -4671,7 +4663,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E151" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F151" s="1">
         <v>0.58333333333333404</v>
@@ -4681,7 +4673,7 @@
       </c>
       <c r="K151" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (150,22,3,'{Judge3}','2023-06-23','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (150,22,3,'{Judge3}','2023-06-24','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
@@ -4699,7 +4691,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E152" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F152" s="1">
         <v>0.625</v>
@@ -4709,7 +4701,7 @@
       </c>
       <c r="K152" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (151,23,3,'{Judge3}','2023-06-23','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (151,23,3,'{Judge3}','2023-06-24','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
@@ -4727,7 +4719,7 @@
         <v>{Judge3}</v>
       </c>
       <c r="E153" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F153" s="1">
         <v>0.66666666666666696</v>
@@ -4737,7 +4729,7 @@
       </c>
       <c r="K153" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (152,24,3,'{Judge3}','2023-06-23','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (152,24,3,'{Judge3}','2023-06-24','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
@@ -4755,7 +4747,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E154" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F154" s="1">
         <v>0.375</v>
@@ -4765,7 +4757,7 @@
       </c>
       <c r="K154" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (153,25,4,'{Judge4}','2023-06-23','09:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (153,25,4,'{Judge4}','2023-06-24','09:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
@@ -4783,7 +4775,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E155" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F155" s="1">
         <v>0.41666666666666669</v>
@@ -4793,7 +4785,7 @@
       </c>
       <c r="K155" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (154,26,4,'{Judge4}','2023-06-23','10:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (154,26,4,'{Judge4}','2023-06-24','10:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
@@ -4811,7 +4803,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E156" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F156" s="1">
         <v>0.45833333333333331</v>
@@ -4821,7 +4813,7 @@
       </c>
       <c r="K156" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (155,27,4,'{Judge4}','2023-06-23','11:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (155,27,4,'{Judge4}','2023-06-24','11:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
@@ -4839,7 +4831,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E157" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F157" s="1">
         <v>0.5</v>
@@ -4849,7 +4841,7 @@
       </c>
       <c r="K157" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (156,28,4,'{Judge4}','2023-06-23','12:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (156,28,4,'{Judge4}','2023-06-24','12:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
@@ -4867,7 +4859,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E158" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F158" s="1">
         <v>0.54166666666666696</v>
@@ -4877,7 +4869,7 @@
       </c>
       <c r="K158" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (157,29,4,'{Judge4}','2023-06-23','13:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (157,29,4,'{Judge4}','2023-06-24','13:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
@@ -4895,7 +4887,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E159" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F159" s="1">
         <v>0.58333333333333404</v>
@@ -4905,7 +4897,7 @@
       </c>
       <c r="K159" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (158,30,4,'{Judge4}','2023-06-23','14:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (158,30,4,'{Judge4}','2023-06-24','14:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
@@ -4923,7 +4915,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E160" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F160" s="1">
         <v>0.625</v>
@@ -4933,7 +4925,7 @@
       </c>
       <c r="K160" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (159,31,4,'{Judge4}','2023-06-23','15:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (159,31,4,'{Judge4}','2023-06-24','15:00:00',TRUE, NULL);</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
@@ -4951,7 +4943,7 @@
         <v>{Judge4}</v>
       </c>
       <c r="E161" s="2">
-        <v>45100</v>
+        <v>45101</v>
       </c>
       <c r="F161" s="1">
         <v>0.66666666666666696</v>
@@ -4961,7 +4953,7 @@
       </c>
       <c r="K161" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO moj_hearing VALUES (160,32,4,'{Judge4}','2023-06-23','16:00:00',TRUE, NULL);</v>
+        <v>INSERT INTO moj_hearing VALUES (160,32,4,'{Judge4}','2023-06-24','16:00:00',TRUE, NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -4972,19 +4964,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AD3C3F-6516-434E-8872-39F76B4E1EEA}">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R33"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5021,814 +5013,805 @@
       <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="E2" t="str">
+      <c r="D2" t="str">
         <f>"Case"&amp;TEXT(A2,"0000000")</f>
         <v>Case0000001</v>
       </c>
-      <c r="I2" t="str">
+      <c r="H2" t="str">
         <f>"ARRAY ['Mr Defendant"&amp;TEXT($A2,"0000000")&amp;" Bloggs1','Mr Defendant"&amp;TEXT($A2,"0000000")&amp;" Bloggs2']"</f>
         <v>ARRAY ['Mr Defendant0000001 Bloggs1','Mr Defendant0000001 Bloggs2']</v>
       </c>
-      <c r="J2" t="str">
+      <c r="I2" t="str">
         <f>"ARRAY ['Prosecutor"&amp;TEXT($A2,"0000000")&amp;"1','Prosecutor"&amp;TEXT($A2,"0000000")&amp;"2']"</f>
         <v>ARRAY ['Prosecutor00000011','Prosecutor00000012']</v>
       </c>
-      <c r="K2" t="str">
+      <c r="J2" t="str">
         <f>"ARRAY ['Defence"&amp;TEXT($A2,"0000000")&amp;"1','Defence"&amp;TEXT($A2,"0000000")&amp;"2']"</f>
         <v>ARRAY ['Defence00000011','Defence00000012']</v>
       </c>
-      <c r="R2" t="str">
-        <f>"INSERT INTO moj_case VALUES ("&amp;A2&amp;","&amp;IF(B2="","null",B2)&amp;","&amp;IF(C2="","null",C2)&amp;","&amp;IF(D2="","null",D2)&amp;",'"&amp;E2&amp;"',"&amp;IF(F2="","null",F2)&amp;","&amp;IF(G2="","null",G2)&amp;","&amp;IF(H2="","null",H2)&amp;","&amp;I2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;IF(L2="","null",L2)&amp;","&amp;IF(M2="","null",M2)&amp;","&amp;IF(N2="","null",N2)&amp;","&amp;IF(O2="","null",O2)&amp;");"</f>
-        <v>INSERT INTO moj_case VALUES (1,null,null,null,'Case0000001',null,null,null,ARRAY ['Mr Defendant0000001 Bloggs1','Mr Defendant0000001 Bloggs2'],ARRAY ['Prosecutor00000011','Prosecutor00000012'],ARRAY ['Defence00000011','Defence00000012'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O2" t="str">
+        <f>"INSERT INTO moj_case VALUES ("&amp;A2&amp;","&amp;IF(B2="","null",B2)&amp;","&amp;IF(C2="","null",C2)&amp;",'"&amp;D2&amp;"',"&amp;IF(E2="","null",E2)&amp;","&amp;IF(F2="","null",F2)&amp;","&amp;IF(G2="","null",G2)&amp;","&amp;H2&amp;","&amp;I2&amp;","&amp;J2&amp;","&amp;IF(K2="","null",K2)&amp;","&amp;IF(L2="","null",L2)&amp;");"</f>
+        <v>INSERT INTO moj_case VALUES (1,null,null,'Case0000001',null,null,null,ARRAY ['Mr Defendant0000001 Bloggs1','Mr Defendant0000001 Bloggs2'],ARRAY ['Prosecutor00000011','Prosecutor00000012'],ARRAY ['Defence00000011','Defence00000012'],null,null);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E33" si="0">"Case"&amp;TEXT(A3,"0000000")</f>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D33" si="0">"Case"&amp;TEXT(A3,"0000000")</f>
         <v>Case0000002</v>
       </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H33" si="1">"ARRAY ['Mr Defendant"&amp;TEXT($A3,"0000000")&amp;" Bloggs1','Mr Defendant"&amp;TEXT($A3,"0000000")&amp;" Bloggs2']"</f>
+        <v>ARRAY ['Mr Defendant0000002 Bloggs1','Mr Defendant0000002 Bloggs2']</v>
+      </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I33" si="1">"ARRAY ['Mr Defendant"&amp;TEXT($A3,"0000000")&amp;" Bloggs1','Mr Defendant"&amp;TEXT($A3,"0000000")&amp;" Bloggs2']"</f>
-        <v>ARRAY ['Mr Defendant0000002 Bloggs1','Mr Defendant0000002 Bloggs2']</v>
+        <f t="shared" ref="I3:I33" si="2">"ARRAY ['Prosecutor"&amp;TEXT($A3,"0000000")&amp;"1','Prosecutor"&amp;TEXT($A3,"0000000")&amp;"2']"</f>
+        <v>ARRAY ['Prosecutor00000021','Prosecutor00000022']</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J33" si="2">"ARRAY ['Prosecutor"&amp;TEXT($A3,"0000000")&amp;"1','Prosecutor"&amp;TEXT($A3,"0000000")&amp;"2']"</f>
-        <v>ARRAY ['Prosecutor00000021','Prosecutor00000022']</v>
-      </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K33" si="3">"ARRAY ['Defence"&amp;TEXT($A3,"0000000")&amp;"1','Defence"&amp;TEXT($A3,"0000000")&amp;"2']"</f>
+        <f t="shared" ref="J3:J33" si="3">"ARRAY ['Defence"&amp;TEXT($A3,"0000000")&amp;"1','Defence"&amp;TEXT($A3,"0000000")&amp;"2']"</f>
         <v>ARRAY ['Defence00000021','Defence00000022']</v>
       </c>
-      <c r="R3" t="str">
-        <f t="shared" ref="R3:R33" si="4">"INSERT INTO moj_case VALUES ("&amp;A3&amp;","&amp;IF(B3="","null",B3)&amp;","&amp;IF(C3="","null",C3)&amp;","&amp;IF(D3="","null",D3)&amp;",'"&amp;E3&amp;"',"&amp;IF(F3="","null",F3)&amp;","&amp;IF(G3="","null",G3)&amp;","&amp;IF(H3="","null",H3)&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;IF(L3="","null",L3)&amp;","&amp;IF(M3="","null",M3)&amp;","&amp;IF(N3="","null",N3)&amp;","&amp;IF(O3="","null",O3)&amp;");"</f>
-        <v>INSERT INTO moj_case VALUES (2,null,null,null,'Case0000002',null,null,null,ARRAY ['Mr Defendant0000002 Bloggs1','Mr Defendant0000002 Bloggs2'],ARRAY ['Prosecutor00000021','Prosecutor00000022'],ARRAY ['Defence00000021','Defence00000022'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O33" si="4">"INSERT INTO moj_case VALUES ("&amp;A3&amp;","&amp;IF(B3="","null",B3)&amp;","&amp;IF(C3="","null",C3)&amp;",'"&amp;D3&amp;"',"&amp;IF(E3="","null",E3)&amp;","&amp;IF(F3="","null",F3)&amp;","&amp;IF(G3="","null",G3)&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;IF(K3="","null",K3)&amp;","&amp;IF(L3="","null",L3)&amp;");"</f>
+        <v>INSERT INTO moj_case VALUES (2,null,null,'Case0000002',null,null,null,ARRAY ['Mr Defendant0000002 Bloggs1','Mr Defendant0000002 Bloggs2'],ARRAY ['Prosecutor00000021','Prosecutor00000022'],ARRAY ['Defence00000021','Defence00000022'],null,null);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="E4" t="str">
+      <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>Case0000003</v>
       </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000003 Bloggs1','Mr Defendant0000003 Bloggs2']</v>
+      </c>
       <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000003 Bloggs1','Mr Defendant0000003 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000031','Prosecutor00000032']</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000031','Prosecutor00000032']</v>
-      </c>
-      <c r="K4" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000031','Defence00000032']</v>
       </c>
-      <c r="R4" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (3,null,null,null,'Case0000003',null,null,null,ARRAY ['Mr Defendant0000003 Bloggs1','Mr Defendant0000003 Bloggs2'],ARRAY ['Prosecutor00000031','Prosecutor00000032'],ARRAY ['Defence00000031','Defence00000032'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O4" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (3,null,null,'Case0000003',null,null,null,ARRAY ['Mr Defendant0000003 Bloggs1','Mr Defendant0000003 Bloggs2'],ARRAY ['Prosecutor00000031','Prosecutor00000032'],ARRAY ['Defence00000031','Defence00000032'],null,null);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="E5" t="str">
+      <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>Case0000004</v>
       </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000004 Bloggs1','Mr Defendant0000004 Bloggs2']</v>
+      </c>
       <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000004 Bloggs1','Mr Defendant0000004 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000041','Prosecutor00000042']</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000041','Prosecutor00000042']</v>
-      </c>
-      <c r="K5" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000041','Defence00000042']</v>
       </c>
-      <c r="R5" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (4,null,null,null,'Case0000004',null,null,null,ARRAY ['Mr Defendant0000004 Bloggs1','Mr Defendant0000004 Bloggs2'],ARRAY ['Prosecutor00000041','Prosecutor00000042'],ARRAY ['Defence00000041','Defence00000042'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O5" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (4,null,null,'Case0000004',null,null,null,ARRAY ['Mr Defendant0000004 Bloggs1','Mr Defendant0000004 Bloggs2'],ARRAY ['Prosecutor00000041','Prosecutor00000042'],ARRAY ['Defence00000041','Defence00000042'],null,null);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="E6" t="str">
+      <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Case0000005</v>
       </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000005 Bloggs1','Mr Defendant0000005 Bloggs2']</v>
+      </c>
       <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000005 Bloggs1','Mr Defendant0000005 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000051','Prosecutor00000052']</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000051','Prosecutor00000052']</v>
-      </c>
-      <c r="K6" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000051','Defence00000052']</v>
       </c>
-      <c r="R6" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (5,null,null,null,'Case0000005',null,null,null,ARRAY ['Mr Defendant0000005 Bloggs1','Mr Defendant0000005 Bloggs2'],ARRAY ['Prosecutor00000051','Prosecutor00000052'],ARRAY ['Defence00000051','Defence00000052'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O6" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (5,null,null,'Case0000005',null,null,null,ARRAY ['Mr Defendant0000005 Bloggs1','Mr Defendant0000005 Bloggs2'],ARRAY ['Prosecutor00000051','Prosecutor00000052'],ARRAY ['Defence00000051','Defence00000052'],null,null);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="E7" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>Case0000006</v>
       </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000006 Bloggs1','Mr Defendant0000006 Bloggs2']</v>
+      </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000006 Bloggs1','Mr Defendant0000006 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000061','Prosecutor00000062']</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000061','Prosecutor00000062']</v>
-      </c>
-      <c r="K7" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000061','Defence00000062']</v>
       </c>
-      <c r="R7" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (6,null,null,null,'Case0000006',null,null,null,ARRAY ['Mr Defendant0000006 Bloggs1','Mr Defendant0000006 Bloggs2'],ARRAY ['Prosecutor00000061','Prosecutor00000062'],ARRAY ['Defence00000061','Defence00000062'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O7" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (6,null,null,'Case0000006',null,null,null,ARRAY ['Mr Defendant0000006 Bloggs1','Mr Defendant0000006 Bloggs2'],ARRAY ['Prosecutor00000061','Prosecutor00000062'],ARRAY ['Defence00000061','Defence00000062'],null,null);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="E8" t="str">
+      <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Case0000007</v>
       </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000007 Bloggs1','Mr Defendant0000007 Bloggs2']</v>
+      </c>
       <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000007 Bloggs1','Mr Defendant0000007 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000071','Prosecutor00000072']</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000071','Prosecutor00000072']</v>
-      </c>
-      <c r="K8" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000071','Defence00000072']</v>
       </c>
-      <c r="R8" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (7,null,null,null,'Case0000007',null,null,null,ARRAY ['Mr Defendant0000007 Bloggs1','Mr Defendant0000007 Bloggs2'],ARRAY ['Prosecutor00000071','Prosecutor00000072'],ARRAY ['Defence00000071','Defence00000072'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O8" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (7,null,null,'Case0000007',null,null,null,ARRAY ['Mr Defendant0000007 Bloggs1','Mr Defendant0000007 Bloggs2'],ARRAY ['Prosecutor00000071','Prosecutor00000072'],ARRAY ['Defence00000071','Defence00000072'],null,null);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="E9" t="str">
+      <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Case0000008</v>
       </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000008 Bloggs1','Mr Defendant0000008 Bloggs2']</v>
+      </c>
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000008 Bloggs1','Mr Defendant0000008 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000081','Prosecutor00000082']</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000081','Prosecutor00000082']</v>
-      </c>
-      <c r="K9" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000081','Defence00000082']</v>
       </c>
-      <c r="R9" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (8,null,null,null,'Case0000008',null,null,null,ARRAY ['Mr Defendant0000008 Bloggs1','Mr Defendant0000008 Bloggs2'],ARRAY ['Prosecutor00000081','Prosecutor00000082'],ARRAY ['Defence00000081','Defence00000082'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O9" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (8,null,null,'Case0000008',null,null,null,ARRAY ['Mr Defendant0000008 Bloggs1','Mr Defendant0000008 Bloggs2'],ARRAY ['Prosecutor00000081','Prosecutor00000082'],ARRAY ['Defence00000081','Defence00000082'],null,null);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="E10" t="str">
+      <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>Case0000009</v>
       </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000009 Bloggs1','Mr Defendant0000009 Bloggs2']</v>
+      </c>
       <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000009 Bloggs1','Mr Defendant0000009 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000091','Prosecutor00000092']</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000091','Prosecutor00000092']</v>
-      </c>
-      <c r="K10" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000091','Defence00000092']</v>
       </c>
-      <c r="R10" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (9,null,null,null,'Case0000009',null,null,null,ARRAY ['Mr Defendant0000009 Bloggs1','Mr Defendant0000009 Bloggs2'],ARRAY ['Prosecutor00000091','Prosecutor00000092'],ARRAY ['Defence00000091','Defence00000092'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O10" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (9,null,null,'Case0000009',null,null,null,ARRAY ['Mr Defendant0000009 Bloggs1','Mr Defendant0000009 Bloggs2'],ARRAY ['Prosecutor00000091','Prosecutor00000092'],ARRAY ['Defence00000091','Defence00000092'],null,null);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="E11" t="str">
+      <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>Case0000010</v>
       </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000010 Bloggs1','Mr Defendant0000010 Bloggs2']</v>
+      </c>
       <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000010 Bloggs1','Mr Defendant0000010 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000101','Prosecutor00000102']</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000101','Prosecutor00000102']</v>
-      </c>
-      <c r="K11" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000101','Defence00000102']</v>
       </c>
-      <c r="R11" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (10,null,null,null,'Case0000010',null,null,null,ARRAY ['Mr Defendant0000010 Bloggs1','Mr Defendant0000010 Bloggs2'],ARRAY ['Prosecutor00000101','Prosecutor00000102'],ARRAY ['Defence00000101','Defence00000102'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O11" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (10,null,null,'Case0000010',null,null,null,ARRAY ['Mr Defendant0000010 Bloggs1','Mr Defendant0000010 Bloggs2'],ARRAY ['Prosecutor00000101','Prosecutor00000102'],ARRAY ['Defence00000101','Defence00000102'],null,null);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="E12" t="str">
+      <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Case0000011</v>
       </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000011 Bloggs1','Mr Defendant0000011 Bloggs2']</v>
+      </c>
       <c r="I12" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000011 Bloggs1','Mr Defendant0000011 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000111','Prosecutor00000112']</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000111','Prosecutor00000112']</v>
-      </c>
-      <c r="K12" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000111','Defence00000112']</v>
       </c>
-      <c r="R12" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (11,null,null,null,'Case0000011',null,null,null,ARRAY ['Mr Defendant0000011 Bloggs1','Mr Defendant0000011 Bloggs2'],ARRAY ['Prosecutor00000111','Prosecutor00000112'],ARRAY ['Defence00000111','Defence00000112'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O12" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (11,null,null,'Case0000011',null,null,null,ARRAY ['Mr Defendant0000011 Bloggs1','Mr Defendant0000011 Bloggs2'],ARRAY ['Prosecutor00000111','Prosecutor00000112'],ARRAY ['Defence00000111','Defence00000112'],null,null);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="E13" t="str">
+      <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>Case0000012</v>
       </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000012 Bloggs1','Mr Defendant0000012 Bloggs2']</v>
+      </c>
       <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000012 Bloggs1','Mr Defendant0000012 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000121','Prosecutor00000122']</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000121','Prosecutor00000122']</v>
-      </c>
-      <c r="K13" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000121','Defence00000122']</v>
       </c>
-      <c r="R13" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (12,null,null,null,'Case0000012',null,null,null,ARRAY ['Mr Defendant0000012 Bloggs1','Mr Defendant0000012 Bloggs2'],ARRAY ['Prosecutor00000121','Prosecutor00000122'],ARRAY ['Defence00000121','Defence00000122'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O13" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (12,null,null,'Case0000012',null,null,null,ARRAY ['Mr Defendant0000012 Bloggs1','Mr Defendant0000012 Bloggs2'],ARRAY ['Prosecutor00000121','Prosecutor00000122'],ARRAY ['Defence00000121','Defence00000122'],null,null);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="E14" t="str">
+      <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>Case0000013</v>
       </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000013 Bloggs1','Mr Defendant0000013 Bloggs2']</v>
+      </c>
       <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000013 Bloggs1','Mr Defendant0000013 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000131','Prosecutor00000132']</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000131','Prosecutor00000132']</v>
-      </c>
-      <c r="K14" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000131','Defence00000132']</v>
       </c>
-      <c r="R14" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (13,null,null,null,'Case0000013',null,null,null,ARRAY ['Mr Defendant0000013 Bloggs1','Mr Defendant0000013 Bloggs2'],ARRAY ['Prosecutor00000131','Prosecutor00000132'],ARRAY ['Defence00000131','Defence00000132'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O14" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (13,null,null,'Case0000013',null,null,null,ARRAY ['Mr Defendant0000013 Bloggs1','Mr Defendant0000013 Bloggs2'],ARRAY ['Prosecutor00000131','Prosecutor00000132'],ARRAY ['Defence00000131','Defence00000132'],null,null);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="E15" t="str">
+      <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>Case0000014</v>
       </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000014 Bloggs1','Mr Defendant0000014 Bloggs2']</v>
+      </c>
       <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000014 Bloggs1','Mr Defendant0000014 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000141','Prosecutor00000142']</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000141','Prosecutor00000142']</v>
-      </c>
-      <c r="K15" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000141','Defence00000142']</v>
       </c>
-      <c r="R15" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (14,null,null,null,'Case0000014',null,null,null,ARRAY ['Mr Defendant0000014 Bloggs1','Mr Defendant0000014 Bloggs2'],ARRAY ['Prosecutor00000141','Prosecutor00000142'],ARRAY ['Defence00000141','Defence00000142'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O15" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (14,null,null,'Case0000014',null,null,null,ARRAY ['Mr Defendant0000014 Bloggs1','Mr Defendant0000014 Bloggs2'],ARRAY ['Prosecutor00000141','Prosecutor00000142'],ARRAY ['Defence00000141','Defence00000142'],null,null);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="E16" t="str">
+      <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>Case0000015</v>
       </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000015 Bloggs1','Mr Defendant0000015 Bloggs2']</v>
+      </c>
       <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000015 Bloggs1','Mr Defendant0000015 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000151','Prosecutor00000152']</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000151','Prosecutor00000152']</v>
-      </c>
-      <c r="K16" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000151','Defence00000152']</v>
       </c>
-      <c r="R16" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (15,null,null,null,'Case0000015',null,null,null,ARRAY ['Mr Defendant0000015 Bloggs1','Mr Defendant0000015 Bloggs2'],ARRAY ['Prosecutor00000151','Prosecutor00000152'],ARRAY ['Defence00000151','Defence00000152'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O16" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (15,null,null,'Case0000015',null,null,null,ARRAY ['Mr Defendant0000015 Bloggs1','Mr Defendant0000015 Bloggs2'],ARRAY ['Prosecutor00000151','Prosecutor00000152'],ARRAY ['Defence00000151','Defence00000152'],null,null);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="E17" t="str">
+      <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>Case0000016</v>
       </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000016 Bloggs1','Mr Defendant0000016 Bloggs2']</v>
+      </c>
       <c r="I17" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000016 Bloggs1','Mr Defendant0000016 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000161','Prosecutor00000162']</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000161','Prosecutor00000162']</v>
-      </c>
-      <c r="K17" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000161','Defence00000162']</v>
       </c>
-      <c r="R17" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (16,null,null,null,'Case0000016',null,null,null,ARRAY ['Mr Defendant0000016 Bloggs1','Mr Defendant0000016 Bloggs2'],ARRAY ['Prosecutor00000161','Prosecutor00000162'],ARRAY ['Defence00000161','Defence00000162'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O17" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (16,null,null,'Case0000016',null,null,null,ARRAY ['Mr Defendant0000016 Bloggs1','Mr Defendant0000016 Bloggs2'],ARRAY ['Prosecutor00000161','Prosecutor00000162'],ARRAY ['Defence00000161','Defence00000162'],null,null);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="E18" t="str">
+      <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>Case0000017</v>
       </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000017 Bloggs1','Mr Defendant0000017 Bloggs2']</v>
+      </c>
       <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000017 Bloggs1','Mr Defendant0000017 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000171','Prosecutor00000172']</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000171','Prosecutor00000172']</v>
-      </c>
-      <c r="K18" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000171','Defence00000172']</v>
       </c>
-      <c r="R18" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (17,null,null,null,'Case0000017',null,null,null,ARRAY ['Mr Defendant0000017 Bloggs1','Mr Defendant0000017 Bloggs2'],ARRAY ['Prosecutor00000171','Prosecutor00000172'],ARRAY ['Defence00000171','Defence00000172'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O18" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (17,null,null,'Case0000017',null,null,null,ARRAY ['Mr Defendant0000017 Bloggs1','Mr Defendant0000017 Bloggs2'],ARRAY ['Prosecutor00000171','Prosecutor00000172'],ARRAY ['Defence00000171','Defence00000172'],null,null);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="E19" t="str">
+      <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>Case0000018</v>
       </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000018 Bloggs1','Mr Defendant0000018 Bloggs2']</v>
+      </c>
       <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000018 Bloggs1','Mr Defendant0000018 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000181','Prosecutor00000182']</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000181','Prosecutor00000182']</v>
-      </c>
-      <c r="K19" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000181','Defence00000182']</v>
       </c>
-      <c r="R19" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (18,null,null,null,'Case0000018',null,null,null,ARRAY ['Mr Defendant0000018 Bloggs1','Mr Defendant0000018 Bloggs2'],ARRAY ['Prosecutor00000181','Prosecutor00000182'],ARRAY ['Defence00000181','Defence00000182'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O19" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (18,null,null,'Case0000018',null,null,null,ARRAY ['Mr Defendant0000018 Bloggs1','Mr Defendant0000018 Bloggs2'],ARRAY ['Prosecutor00000181','Prosecutor00000182'],ARRAY ['Defence00000181','Defence00000182'],null,null);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="E20" t="str">
+      <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>Case0000019</v>
       </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000019 Bloggs1','Mr Defendant0000019 Bloggs2']</v>
+      </c>
       <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000019 Bloggs1','Mr Defendant0000019 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000191','Prosecutor00000192']</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000191','Prosecutor00000192']</v>
-      </c>
-      <c r="K20" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000191','Defence00000192']</v>
       </c>
-      <c r="R20" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (19,null,null,null,'Case0000019',null,null,null,ARRAY ['Mr Defendant0000019 Bloggs1','Mr Defendant0000019 Bloggs2'],ARRAY ['Prosecutor00000191','Prosecutor00000192'],ARRAY ['Defence00000191','Defence00000192'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O20" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (19,null,null,'Case0000019',null,null,null,ARRAY ['Mr Defendant0000019 Bloggs1','Mr Defendant0000019 Bloggs2'],ARRAY ['Prosecutor00000191','Prosecutor00000192'],ARRAY ['Defence00000191','Defence00000192'],null,null);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="E21" t="str">
+      <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>Case0000020</v>
       </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000020 Bloggs1','Mr Defendant0000020 Bloggs2']</v>
+      </c>
       <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000020 Bloggs1','Mr Defendant0000020 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000201','Prosecutor00000202']</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000201','Prosecutor00000202']</v>
-      </c>
-      <c r="K21" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000201','Defence00000202']</v>
       </c>
-      <c r="R21" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (20,null,null,null,'Case0000020',null,null,null,ARRAY ['Mr Defendant0000020 Bloggs1','Mr Defendant0000020 Bloggs2'],ARRAY ['Prosecutor00000201','Prosecutor00000202'],ARRAY ['Defence00000201','Defence00000202'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O21" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (20,null,null,'Case0000020',null,null,null,ARRAY ['Mr Defendant0000020 Bloggs1','Mr Defendant0000020 Bloggs2'],ARRAY ['Prosecutor00000201','Prosecutor00000202'],ARRAY ['Defence00000201','Defence00000202'],null,null);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="E22" t="str">
+      <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>Case0000021</v>
       </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000021 Bloggs1','Mr Defendant0000021 Bloggs2']</v>
+      </c>
       <c r="I22" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000021 Bloggs1','Mr Defendant0000021 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000211','Prosecutor00000212']</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000211','Prosecutor00000212']</v>
-      </c>
-      <c r="K22" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000211','Defence00000212']</v>
       </c>
-      <c r="R22" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (21,null,null,null,'Case0000021',null,null,null,ARRAY ['Mr Defendant0000021 Bloggs1','Mr Defendant0000021 Bloggs2'],ARRAY ['Prosecutor00000211','Prosecutor00000212'],ARRAY ['Defence00000211','Defence00000212'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O22" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (21,null,null,'Case0000021',null,null,null,ARRAY ['Mr Defendant0000021 Bloggs1','Mr Defendant0000021 Bloggs2'],ARRAY ['Prosecutor00000211','Prosecutor00000212'],ARRAY ['Defence00000211','Defence00000212'],null,null);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="E23" t="str">
+      <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>Case0000022</v>
       </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000022 Bloggs1','Mr Defendant0000022 Bloggs2']</v>
+      </c>
       <c r="I23" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000022 Bloggs1','Mr Defendant0000022 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000221','Prosecutor00000222']</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000221','Prosecutor00000222']</v>
-      </c>
-      <c r="K23" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000221','Defence00000222']</v>
       </c>
-      <c r="R23" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (22,null,null,null,'Case0000022',null,null,null,ARRAY ['Mr Defendant0000022 Bloggs1','Mr Defendant0000022 Bloggs2'],ARRAY ['Prosecutor00000221','Prosecutor00000222'],ARRAY ['Defence00000221','Defence00000222'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O23" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (22,null,null,'Case0000022',null,null,null,ARRAY ['Mr Defendant0000022 Bloggs1','Mr Defendant0000022 Bloggs2'],ARRAY ['Prosecutor00000221','Prosecutor00000222'],ARRAY ['Defence00000221','Defence00000222'],null,null);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="E24" t="str">
+      <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>Case0000023</v>
       </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000023 Bloggs1','Mr Defendant0000023 Bloggs2']</v>
+      </c>
       <c r="I24" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000023 Bloggs1','Mr Defendant0000023 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000231','Prosecutor00000232']</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000231','Prosecutor00000232']</v>
-      </c>
-      <c r="K24" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000231','Defence00000232']</v>
       </c>
-      <c r="R24" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (23,null,null,null,'Case0000023',null,null,null,ARRAY ['Mr Defendant0000023 Bloggs1','Mr Defendant0000023 Bloggs2'],ARRAY ['Prosecutor00000231','Prosecutor00000232'],ARRAY ['Defence00000231','Defence00000232'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O24" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (23,null,null,'Case0000023',null,null,null,ARRAY ['Mr Defendant0000023 Bloggs1','Mr Defendant0000023 Bloggs2'],ARRAY ['Prosecutor00000231','Prosecutor00000232'],ARRAY ['Defence00000231','Defence00000232'],null,null);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="E25" t="str">
+      <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>Case0000024</v>
       </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000024 Bloggs1','Mr Defendant0000024 Bloggs2']</v>
+      </c>
       <c r="I25" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000024 Bloggs1','Mr Defendant0000024 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000241','Prosecutor00000242']</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000241','Prosecutor00000242']</v>
-      </c>
-      <c r="K25" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000241','Defence00000242']</v>
       </c>
-      <c r="R25" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (24,null,null,null,'Case0000024',null,null,null,ARRAY ['Mr Defendant0000024 Bloggs1','Mr Defendant0000024 Bloggs2'],ARRAY ['Prosecutor00000241','Prosecutor00000242'],ARRAY ['Defence00000241','Defence00000242'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O25" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (24,null,null,'Case0000024',null,null,null,ARRAY ['Mr Defendant0000024 Bloggs1','Mr Defendant0000024 Bloggs2'],ARRAY ['Prosecutor00000241','Prosecutor00000242'],ARRAY ['Defence00000241','Defence00000242'],null,null);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="E26" t="str">
+      <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>Case0000025</v>
       </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000025 Bloggs1','Mr Defendant0000025 Bloggs2']</v>
+      </c>
       <c r="I26" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000025 Bloggs1','Mr Defendant0000025 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000251','Prosecutor00000252']</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000251','Prosecutor00000252']</v>
-      </c>
-      <c r="K26" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000251','Defence00000252']</v>
       </c>
-      <c r="R26" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (25,null,null,null,'Case0000025',null,null,null,ARRAY ['Mr Defendant0000025 Bloggs1','Mr Defendant0000025 Bloggs2'],ARRAY ['Prosecutor00000251','Prosecutor00000252'],ARRAY ['Defence00000251','Defence00000252'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O26" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (25,null,null,'Case0000025',null,null,null,ARRAY ['Mr Defendant0000025 Bloggs1','Mr Defendant0000025 Bloggs2'],ARRAY ['Prosecutor00000251','Prosecutor00000252'],ARRAY ['Defence00000251','Defence00000252'],null,null);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="E27" t="str">
+      <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>Case0000026</v>
       </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000026 Bloggs1','Mr Defendant0000026 Bloggs2']</v>
+      </c>
       <c r="I27" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000026 Bloggs1','Mr Defendant0000026 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000261','Prosecutor00000262']</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000261','Prosecutor00000262']</v>
-      </c>
-      <c r="K27" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000261','Defence00000262']</v>
       </c>
-      <c r="R27" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (26,null,null,null,'Case0000026',null,null,null,ARRAY ['Mr Defendant0000026 Bloggs1','Mr Defendant0000026 Bloggs2'],ARRAY ['Prosecutor00000261','Prosecutor00000262'],ARRAY ['Defence00000261','Defence00000262'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O27" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (26,null,null,'Case0000026',null,null,null,ARRAY ['Mr Defendant0000026 Bloggs1','Mr Defendant0000026 Bloggs2'],ARRAY ['Prosecutor00000261','Prosecutor00000262'],ARRAY ['Defence00000261','Defence00000262'],null,null);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="E28" t="str">
+      <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>Case0000027</v>
       </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000027 Bloggs1','Mr Defendant0000027 Bloggs2']</v>
+      </c>
       <c r="I28" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000027 Bloggs1','Mr Defendant0000027 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000271','Prosecutor00000272']</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000271','Prosecutor00000272']</v>
-      </c>
-      <c r="K28" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000271','Defence00000272']</v>
       </c>
-      <c r="R28" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (27,null,null,null,'Case0000027',null,null,null,ARRAY ['Mr Defendant0000027 Bloggs1','Mr Defendant0000027 Bloggs2'],ARRAY ['Prosecutor00000271','Prosecutor00000272'],ARRAY ['Defence00000271','Defence00000272'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O28" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (27,null,null,'Case0000027',null,null,null,ARRAY ['Mr Defendant0000027 Bloggs1','Mr Defendant0000027 Bloggs2'],ARRAY ['Prosecutor00000271','Prosecutor00000272'],ARRAY ['Defence00000271','Defence00000272'],null,null);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="E29" t="str">
+      <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>Case0000028</v>
       </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000028 Bloggs1','Mr Defendant0000028 Bloggs2']</v>
+      </c>
       <c r="I29" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000028 Bloggs1','Mr Defendant0000028 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000281','Prosecutor00000282']</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000281','Prosecutor00000282']</v>
-      </c>
-      <c r="K29" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000281','Defence00000282']</v>
       </c>
-      <c r="R29" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (28,null,null,null,'Case0000028',null,null,null,ARRAY ['Mr Defendant0000028 Bloggs1','Mr Defendant0000028 Bloggs2'],ARRAY ['Prosecutor00000281','Prosecutor00000282'],ARRAY ['Defence00000281','Defence00000282'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O29" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (28,null,null,'Case0000028',null,null,null,ARRAY ['Mr Defendant0000028 Bloggs1','Mr Defendant0000028 Bloggs2'],ARRAY ['Prosecutor00000281','Prosecutor00000282'],ARRAY ['Defence00000281','Defence00000282'],null,null);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="E30" t="str">
+      <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>Case0000029</v>
       </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000029 Bloggs1','Mr Defendant0000029 Bloggs2']</v>
+      </c>
       <c r="I30" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000029 Bloggs1','Mr Defendant0000029 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000291','Prosecutor00000292']</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000291','Prosecutor00000292']</v>
-      </c>
-      <c r="K30" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000291','Defence00000292']</v>
       </c>
-      <c r="R30" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (29,null,null,null,'Case0000029',null,null,null,ARRAY ['Mr Defendant0000029 Bloggs1','Mr Defendant0000029 Bloggs2'],ARRAY ['Prosecutor00000291','Prosecutor00000292'],ARRAY ['Defence00000291','Defence00000292'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O30" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (29,null,null,'Case0000029',null,null,null,ARRAY ['Mr Defendant0000029 Bloggs1','Mr Defendant0000029 Bloggs2'],ARRAY ['Prosecutor00000291','Prosecutor00000292'],ARRAY ['Defence00000291','Defence00000292'],null,null);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="E31" t="str">
+      <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>Case0000030</v>
       </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000030 Bloggs1','Mr Defendant0000030 Bloggs2']</v>
+      </c>
       <c r="I31" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000030 Bloggs1','Mr Defendant0000030 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000301','Prosecutor00000302']</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000301','Prosecutor00000302']</v>
-      </c>
-      <c r="K31" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000301','Defence00000302']</v>
       </c>
-      <c r="R31" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (30,null,null,null,'Case0000030',null,null,null,ARRAY ['Mr Defendant0000030 Bloggs1','Mr Defendant0000030 Bloggs2'],ARRAY ['Prosecutor00000301','Prosecutor00000302'],ARRAY ['Defence00000301','Defence00000302'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O31" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (30,null,null,'Case0000030',null,null,null,ARRAY ['Mr Defendant0000030 Bloggs1','Mr Defendant0000030 Bloggs2'],ARRAY ['Prosecutor00000301','Prosecutor00000302'],ARRAY ['Defence00000301','Defence00000302'],null,null);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="E32" t="str">
+      <c r="D32" t="str">
         <f t="shared" si="0"/>
         <v>Case0000031</v>
       </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000031 Bloggs1','Mr Defendant0000031 Bloggs2']</v>
+      </c>
       <c r="I32" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000031 Bloggs1','Mr Defendant0000031 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000311','Prosecutor00000312']</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000311','Prosecutor00000312']</v>
-      </c>
-      <c r="K32" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000311','Defence00000312']</v>
       </c>
-      <c r="R32" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (31,null,null,null,'Case0000031',null,null,null,ARRAY ['Mr Defendant0000031 Bloggs1','Mr Defendant0000031 Bloggs2'],ARRAY ['Prosecutor00000311','Prosecutor00000312'],ARRAY ['Defence00000311','Defence00000312'],null,null,null,null);</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O32" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (31,null,null,'Case0000031',null,null,null,ARRAY ['Mr Defendant0000031 Bloggs1','Mr Defendant0000031 Bloggs2'],ARRAY ['Prosecutor00000311','Prosecutor00000312'],ARRAY ['Defence00000311','Defence00000312'],null,null);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="E33" t="str">
+      <c r="D33" t="str">
         <f t="shared" si="0"/>
         <v>Case0000032</v>
       </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>ARRAY ['Mr Defendant0000032 Bloggs1','Mr Defendant0000032 Bloggs2']</v>
+      </c>
       <c r="I33" t="str">
-        <f t="shared" si="1"/>
-        <v>ARRAY ['Mr Defendant0000032 Bloggs1','Mr Defendant0000032 Bloggs2']</v>
+        <f t="shared" si="2"/>
+        <v>ARRAY ['Prosecutor00000321','Prosecutor00000322']</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="2"/>
-        <v>ARRAY ['Prosecutor00000321','Prosecutor00000322']</v>
-      </c>
-      <c r="K33" t="str">
         <f t="shared" si="3"/>
         <v>ARRAY ['Defence00000321','Defence00000322']</v>
       </c>
-      <c r="R33" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO moj_case VALUES (32,null,null,null,'Case0000032',null,null,null,ARRAY ['Mr Defendant0000032 Bloggs1','Mr Defendant0000032 Bloggs2'],ARRAY ['Prosecutor00000321','Prosecutor00000322'],ARRAY ['Defence00000321','Defence00000322'],null,null,null,null);</v>
+      <c r="O33" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO moj_case VALUES (32,null,null,'Case0000032',null,null,null,ARRAY ['Mr Defendant0000032 Bloggs1','Mr Defendant0000032 Bloggs2'],ARRAY ['Prosecutor00000321','Prosecutor00000322'],ARRAY ['Defence00000321','Defence00000322'],null,null);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>